<commit_message>
commit refactor code v3
</commit_message>
<xml_diff>
--- a/src/main/resources/config_1.xlsx
+++ b/src/main/resources/config_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2364" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2364" windowHeight="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
   <si>
     <t>fields</t>
   </si>
@@ -101,205 +101,109 @@
     <t>Day_Name</t>
   </si>
   <si>
+    <t>Start_Date_Time</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>End_Date_Time</t>
+  </si>
+  <si>
+    <t>Reason_Code</t>
+  </si>
+  <si>
+    <t>Reason_Description</t>
+  </si>
+  <si>
+    <t>Sick Leave |Personal Leave |Vacation Leave</t>
+  </si>
+  <si>
+    <t>Date_Time_To</t>
+  </si>
+  <si>
+    <t>Work_Schedule_ID</t>
+  </si>
+  <si>
+    <t>FFFF</t>
+  </si>
+  <si>
+    <t>LLLL</t>
+  </si>
+  <si>
+    <t>MMMM</t>
+  </si>
+  <si>
+    <t>Male|Female</t>
+  </si>
+  <si>
+    <t>DETAIL</t>
+  </si>
+  <si>
+    <t>Programmer|Tester|UX/UI|DataScience|DataEngineer</t>
+  </si>
+  <si>
+    <t>S|P|V</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD HH:MM:SS</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Start_Time</t>
+  </si>
+  <si>
+    <t>End_Time</t>
+  </si>
+  <si>
+    <t>WW0002</t>
+  </si>
+  <si>
+    <t>WW0003</t>
+  </si>
+  <si>
+    <t>WW0004</t>
+  </si>
+  <si>
+    <t>WW0005</t>
+  </si>
+  <si>
+    <t>WW0006</t>
+  </si>
+  <si>
+    <t>WW0007</t>
+  </si>
+  <si>
+    <t>WW0008</t>
+  </si>
+  <si>
+    <t>WW0009</t>
+  </si>
+  <si>
+    <t>TIME</t>
+  </si>
+  <si>
+    <t>EM0002</t>
+  </si>
+  <si>
+    <t>EM0003</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Date_Time_From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other_Details </t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
     <t>Sunday|Monday|Tuesday|Wednesday|Thursday|Friday|Saturday</t>
-  </si>
-  <si>
-    <t>Start_Date_Time</t>
-  </si>
-  <si>
-    <t>DateTime</t>
-  </si>
-  <si>
-    <t>End_Date_Time</t>
-  </si>
-  <si>
-    <t>Reason_Code</t>
-  </si>
-  <si>
-    <t>Reason_Description</t>
-  </si>
-  <si>
-    <t>Sick Leave |Personal Leave |Vacation Leave</t>
-  </si>
-  <si>
-    <t>Date_Time_from</t>
-  </si>
-  <si>
-    <t>Date_Time_To</t>
-  </si>
-  <si>
-    <t>Work_Schedule_ID</t>
-  </si>
-  <si>
-    <t>FFFF</t>
-  </si>
-  <si>
-    <t>LLLL</t>
-  </si>
-  <si>
-    <t>MMMM</t>
-  </si>
-  <si>
-    <t>Male|Female</t>
-  </si>
-  <si>
-    <t>DETAIL</t>
-  </si>
-  <si>
-    <t>Programmer|Tester|UX/UI|DataScience|DataEngineer</t>
-  </si>
-  <si>
-    <t>S|P|V</t>
-  </si>
-  <si>
-    <t>YYYY:MM:DD</t>
-  </si>
-  <si>
-    <t>YYYY-MM-DD HH:MM:SS</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Start_Time</t>
-  </si>
-  <si>
-    <t>End_Time</t>
-  </si>
-  <si>
-    <t>HH:MM:SS</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>th</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>01-01-2020  7:00:00</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>day_name</t>
-  </si>
-  <si>
-    <t>st</t>
-  </si>
-  <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>oth</t>
-  </si>
-  <si>
-    <t>01-01-2020  15:00:00</t>
-  </si>
-  <si>
-    <t>01-01-2020  23:00:00</t>
-  </si>
-  <si>
-    <t>02-01-2020  23:00:00</t>
-  </si>
-  <si>
-    <t>02-01-2020  07:00:00</t>
-  </si>
-  <si>
-    <t>02-01-2020  7:00:00</t>
-  </si>
-  <si>
-    <t>02-01-2020  15:00:00</t>
-  </si>
-  <si>
-    <t>03-01-2020  23:00:00</t>
-  </si>
-  <si>
-    <t>03-01-2020  07:00:00</t>
-  </si>
-  <si>
-    <t>03-01-2020  7:00:00</t>
-  </si>
-  <si>
-    <t>03-01-2020  15:00:00</t>
-  </si>
-  <si>
-    <t>04-01-2020  23:00:00</t>
-  </si>
-  <si>
-    <t>04-01-2020  07:00:00</t>
-  </si>
-  <si>
-    <t>04-01-2020  15:00:00</t>
-  </si>
-  <si>
-    <t>04-01-2020  7:00:00</t>
-  </si>
-  <si>
-    <t>05-01-2020  23:00:00</t>
-  </si>
-  <si>
-    <t>05-01-2020  07:00:00</t>
-  </si>
-  <si>
-    <t>05-01-2020  7:00:00</t>
-  </si>
-  <si>
-    <t>05-01-2020  15:00:00</t>
-  </si>
-  <si>
-    <t>06-01-2020  07:00:00</t>
-  </si>
-  <si>
-    <t>WW0002</t>
-  </si>
-  <si>
-    <t>WW0003</t>
-  </si>
-  <si>
-    <t>WW0004</t>
-  </si>
-  <si>
-    <t>WW0005</t>
-  </si>
-  <si>
-    <t>WW0006</t>
-  </si>
-  <si>
-    <t>WW0007</t>
-  </si>
-  <si>
-    <t>WW0008</t>
-  </si>
-  <si>
-    <t>WW0009</t>
-  </si>
-  <si>
-    <t>WW0010</t>
-  </si>
-  <si>
-    <t>WW0011</t>
-  </si>
-  <si>
-    <t>WW0012</t>
-  </si>
-  <si>
-    <t>WW0013</t>
-  </si>
-  <si>
-    <t>WW0014</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
   </si>
 </sst>
 </file>
@@ -453,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -490,6 +394,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -780,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -851,7 +758,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
@@ -862,7 +769,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
@@ -873,7 +780,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
@@ -884,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
@@ -895,7 +802,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
@@ -906,7 +813,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -922,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" customHeight="1"/>
@@ -983,7 +890,7 @@
         <v>23</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>13</v>
@@ -991,46 +898,46 @@
     </row>
     <row r="6" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1">
       <c r="B6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1">
       <c r="B7" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1">
       <c r="B8" s="13" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1">
       <c r="B9" s="13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="17.399999999999999" customHeight="1" thickBot="1">
@@ -1038,7 +945,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>13</v>
@@ -1055,7 +962,7 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1078,10 +985,10 @@
     </row>
     <row r="2" spans="2:4" ht="18">
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>13</v>
@@ -1089,10 +996,10 @@
     </row>
     <row r="3" spans="2:4" ht="18">
       <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>13</v>
@@ -1111,10 +1018,10 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" s="7" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>14</v>
@@ -1122,10 +1029,10 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -1133,7 +1040,7 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>18</v>
@@ -1147,7 +1054,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>13</v>
@@ -1158,7 +1065,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>13</v>
@@ -1166,384 +1073,225 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="21.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>38</v>
       </c>
+      <c r="D3" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>61</v>
-      </c>
+      <c r="D4" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B5" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>63</v>
-      </c>
+      <c r="D5" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>60</v>
-      </c>
+      <c r="D6" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>65</v>
-      </c>
+      <c r="D7" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="D8" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" ht="12.6" customHeight="1">
       <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C9" t="s">
         <v>38</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.6" customHeight="1">
+      <c r="D9" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>69</v>
-      </c>
+      <c r="D10" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>70</v>
-      </c>
+      <c r="B11" s="20"/>
+      <c r="D11" s="19"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>68</v>
-      </c>
+      <c r="B12" s="20"/>
+      <c r="D12" s="19"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>73</v>
-      </c>
+      <c r="B13" s="20"/>
+      <c r="D13" s="19"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>75</v>
-      </c>
+      <c r="B14" s="20"/>
+      <c r="D14" s="19"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>72</v>
-      </c>
+      <c r="B15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="J16" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="3:5">
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-    </row>
-    <row r="24" spans="3:5">
-      <c r="E24" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+    </row>
+    <row r="23" spans="5:5">
+      <c r="E23" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>